<commit_message>
Dialogues works fine, need testing on more quests, for now just one is done
</commit_message>
<xml_diff>
--- a/data/quest_dialogues_data.xlsx
+++ b/data/quest_dialogues_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marcin\Desktop\pygame\Kolo_game\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C869FFF1-722E-4102-9DB8-3B0AB23B6D53}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{330855B8-B28E-41C8-AA7B-2B1C4466AF31}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="49">
   <si>
     <t>QuestID</t>
   </si>
@@ -104,11 +104,6 @@
     <t>Give regards from Snorlax</t>
   </si>
   <si>
-    <t>1. Gold+=100
-2. Gold+=100;Item#20
-3. Fight_Init</t>
-  </si>
-  <si>
     <t>Interact</t>
   </si>
   <si>
@@ -121,9 +116,6 @@
     <t>Snorlax:    I need someone to give my regards to Mr. MIME from the castle.</t>
   </si>
   <si>
-    <t>Snorlax:    Farewell!</t>
-  </si>
-  <si>
     <t>Snorlax:    Come back when You fullfill my will.</t>
   </si>
   <si>
@@ -131,12 +123,6 @@
   </si>
   <si>
     <t>Snorlax:    Here's the cash for the quest.</t>
-  </si>
-  <si>
-    <t>Snorlax:    
-1. Cool, here's cash.
-2. Ok, I'll give you item as an extra
-3. Oh shit</t>
   </si>
   <si>
     <t>Mr. Mime:    Hey, How You Doin'?</t>
@@ -162,6 +148,39 @@
     <t>Me:    
 1. I will handle it!
 2. I do not have time for this right now.</t>
+  </si>
+  <si>
+    <t>Choice</t>
+  </si>
+  <si>
+    <t>Snorlax:    Ok, I'll give you sth extra</t>
+  </si>
+  <si>
+    <t>Snorlax:    Oh…. Shit....</t>
+  </si>
+  <si>
+    <t>Snorlax:    1. Cool, here's cash.</t>
+  </si>
+  <si>
+    <t>2. Gold+=100;Item#20</t>
+  </si>
+  <si>
+    <t>3. Fight_Init</t>
+  </si>
+  <si>
+    <t>1. Gold+=100</t>
+  </si>
+  <si>
+    <t>Mr. Mime:    Bye!</t>
+  </si>
+  <si>
+    <t>Snorlax:    You da best! Farewell!</t>
+  </si>
+  <si>
+    <t>Snorlax:    Maybe next time :), Farewell!</t>
+  </si>
+  <si>
+    <t>Me:    See Ya later my friend!</t>
   </si>
 </sst>
 </file>
@@ -602,20 +621,21 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:J15"/>
+  <dimension ref="A1:K20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H18" sqref="H17:H18"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="8" max="8" width="61.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="68.140625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="20.85546875" customWidth="1"/>
     <col min="10" max="10" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="10.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>10</v>
       </c>
@@ -626,7 +646,7 @@
         <v>1</v>
       </c>
       <c r="D1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E1" t="s">
         <v>13</v>
@@ -646,8 +666,11 @@
       <c r="J1" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>111</v>
       </c>
@@ -664,13 +687,16 @@
         <v>1</v>
       </c>
       <c r="H2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="J2" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>111</v>
       </c>
@@ -687,13 +713,13 @@
         <v>2</v>
       </c>
       <c r="H3" t="s">
-        <v>28</v>
-      </c>
-      <c r="J3" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+        <v>27</v>
+      </c>
+      <c r="K3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>111</v>
       </c>
@@ -710,13 +736,13 @@
         <v>3</v>
       </c>
       <c r="H4" t="s">
-        <v>29</v>
-      </c>
-      <c r="J4" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+        <v>28</v>
+      </c>
+      <c r="K4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>111</v>
       </c>
@@ -736,13 +762,13 @@
         <v>2</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="J5" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+        <v>37</v>
+      </c>
+      <c r="K5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>111</v>
       </c>
@@ -759,232 +785,353 @@
         <v>5</v>
       </c>
       <c r="H6" t="s">
+        <v>46</v>
+      </c>
+      <c r="K6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>111</v>
+      </c>
+      <c r="B7">
+        <v>1</v>
+      </c>
+      <c r="C7">
+        <v>0</v>
+      </c>
+      <c r="D7" t="s">
+        <v>15</v>
+      </c>
+      <c r="E7">
+        <v>6</v>
+      </c>
+      <c r="H7" t="s">
+        <v>47</v>
+      </c>
+      <c r="K7">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>111</v>
+      </c>
+      <c r="B8">
+        <v>1</v>
+      </c>
+      <c r="C8">
+        <v>0</v>
+      </c>
+      <c r="D8" t="s">
+        <v>15</v>
+      </c>
+      <c r="E8">
+        <v>7</v>
+      </c>
+      <c r="H8" t="s">
+        <v>48</v>
+      </c>
+      <c r="K8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>111</v>
+      </c>
+      <c r="B9">
+        <v>1</v>
+      </c>
+      <c r="C9">
+        <v>0.5</v>
+      </c>
+      <c r="D9" t="s">
+        <v>15</v>
+      </c>
+      <c r="E9">
+        <v>1</v>
+      </c>
+      <c r="H9" t="s">
+        <v>29</v>
+      </c>
+      <c r="K9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>111</v>
+      </c>
+      <c r="B10">
+        <v>1</v>
+      </c>
+      <c r="C10">
+        <v>2</v>
+      </c>
+      <c r="D10" t="s">
+        <v>15</v>
+      </c>
+      <c r="E10">
+        <v>1</v>
+      </c>
+      <c r="H10" t="s">
         <v>30</v>
       </c>
-      <c r="J6" t="s">
+      <c r="K10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>111</v>
+      </c>
+      <c r="B11">
+        <v>1</v>
+      </c>
+      <c r="C11">
+        <v>2</v>
+      </c>
+      <c r="D11" t="s">
+        <v>15</v>
+      </c>
+      <c r="E11">
+        <v>2</v>
+      </c>
+      <c r="H11" t="s">
+        <v>31</v>
+      </c>
+      <c r="K11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" ht="60" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>111</v>
+      </c>
+      <c r="B12">
+        <v>1</v>
+      </c>
+      <c r="C12">
+        <v>2</v>
+      </c>
+      <c r="D12" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A7">
-        <v>111</v>
-      </c>
-      <c r="B7">
-        <v>1</v>
-      </c>
-      <c r="C7">
-        <v>0.5</v>
-      </c>
-      <c r="D7" t="s">
-        <v>15</v>
-      </c>
-      <c r="E7">
-        <v>1</v>
-      </c>
-      <c r="H7" t="s">
-        <v>31</v>
-      </c>
-      <c r="J7" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A8">
-        <v>111</v>
-      </c>
-      <c r="B8">
-        <v>1</v>
-      </c>
-      <c r="C8">
-        <v>2</v>
-      </c>
-      <c r="D8" t="s">
-        <v>15</v>
-      </c>
-      <c r="E8">
-        <v>1</v>
-      </c>
-      <c r="H8" t="s">
+      <c r="E12">
+        <v>3</v>
+      </c>
+      <c r="F12">
+        <v>3</v>
+      </c>
+      <c r="G12" t="s">
+        <v>20</v>
+      </c>
+      <c r="H12" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="K12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>111</v>
+      </c>
+      <c r="B13">
+        <v>1</v>
+      </c>
+      <c r="C13">
+        <v>2</v>
+      </c>
+      <c r="D13" t="s">
+        <v>15</v>
+      </c>
+      <c r="E13">
+        <v>4</v>
+      </c>
+      <c r="H13" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="I13" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="K13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>111</v>
+      </c>
+      <c r="B14">
+        <v>1</v>
+      </c>
+      <c r="C14">
+        <v>2</v>
+      </c>
+      <c r="D14" t="s">
+        <v>15</v>
+      </c>
+      <c r="E14">
+        <v>5</v>
+      </c>
+      <c r="H14" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="I14" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="K14">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>111</v>
+      </c>
+      <c r="B15">
+        <v>1</v>
+      </c>
+      <c r="C15">
+        <v>2</v>
+      </c>
+      <c r="D15" t="s">
+        <v>15</v>
+      </c>
+      <c r="E15">
+        <v>6</v>
+      </c>
+      <c r="H15" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="I15" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="K15">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>222</v>
+      </c>
+      <c r="B16">
+        <v>0</v>
+      </c>
+      <c r="C16">
+        <v>0</v>
+      </c>
+      <c r="D16" t="s">
+        <v>15</v>
+      </c>
+      <c r="E16">
+        <v>1</v>
+      </c>
+      <c r="H16" t="s">
         <v>32</v>
       </c>
-      <c r="J8" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A9">
-        <v>111</v>
-      </c>
-      <c r="B9">
-        <v>1</v>
-      </c>
-      <c r="C9">
-        <v>2</v>
-      </c>
-      <c r="D9" t="s">
-        <v>15</v>
-      </c>
-      <c r="E9">
-        <v>2</v>
-      </c>
-      <c r="H9" t="s">
+      <c r="J16" t="s">
+        <v>19</v>
+      </c>
+      <c r="K16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>222</v>
+      </c>
+      <c r="B17">
+        <v>0</v>
+      </c>
+      <c r="C17">
+        <v>0</v>
+      </c>
+      <c r="D17" t="s">
+        <v>15</v>
+      </c>
+      <c r="E17">
+        <v>2</v>
+      </c>
+      <c r="H17" t="s">
+        <v>34</v>
+      </c>
+      <c r="K17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>222</v>
+      </c>
+      <c r="B18">
+        <v>1</v>
+      </c>
+      <c r="C18">
+        <v>1</v>
+      </c>
+      <c r="D18" t="s">
+        <v>19</v>
+      </c>
+      <c r="E18">
+        <v>1</v>
+      </c>
+      <c r="F18">
+        <v>2</v>
+      </c>
+      <c r="H18" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="K18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>222</v>
+      </c>
+      <c r="B19">
+        <v>1</v>
+      </c>
+      <c r="C19">
+        <v>1</v>
+      </c>
+      <c r="D19" t="s">
+        <v>15</v>
+      </c>
+      <c r="E19">
+        <v>2</v>
+      </c>
+      <c r="H19" t="s">
         <v>33</v>
       </c>
-      <c r="J9" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" ht="60" x14ac:dyDescent="0.25">
-      <c r="A10">
-        <v>111</v>
-      </c>
-      <c r="B10">
-        <v>1</v>
-      </c>
-      <c r="C10">
-        <v>2</v>
-      </c>
-      <c r="D10" t="s">
-        <v>19</v>
-      </c>
-      <c r="E10">
+      <c r="K19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>222</v>
+      </c>
+      <c r="B20">
+        <v>1</v>
+      </c>
+      <c r="C20">
+        <v>1</v>
+      </c>
+      <c r="D20" t="s">
+        <v>15</v>
+      </c>
+      <c r="E20">
         <v>3</v>
       </c>
-      <c r="F10">
-        <v>3</v>
-      </c>
-      <c r="G10" t="s">
-        <v>20</v>
-      </c>
-      <c r="H10" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="J10" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" ht="60" x14ac:dyDescent="0.25">
-      <c r="A11">
-        <v>111</v>
-      </c>
-      <c r="B11">
-        <v>1</v>
-      </c>
-      <c r="C11">
-        <v>2</v>
-      </c>
-      <c r="D11" t="s">
-        <v>15</v>
-      </c>
-      <c r="E11">
-        <v>4</v>
-      </c>
-      <c r="F11">
-        <v>3</v>
-      </c>
-      <c r="H11" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="I11" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="J11" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A12">
-        <v>222</v>
-      </c>
-      <c r="B12">
-        <v>0</v>
-      </c>
-      <c r="C12">
-        <v>0</v>
-      </c>
-      <c r="D12" t="s">
-        <v>15</v>
-      </c>
-      <c r="E12">
-        <v>1</v>
-      </c>
-      <c r="H12" t="s">
-        <v>35</v>
-      </c>
-      <c r="J12" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A13">
-        <v>222</v>
-      </c>
-      <c r="B13">
-        <v>0</v>
-      </c>
-      <c r="C13">
-        <v>0</v>
-      </c>
-      <c r="D13" t="s">
-        <v>15</v>
-      </c>
-      <c r="E13">
-        <v>2</v>
-      </c>
-      <c r="H13" t="s">
-        <v>37</v>
-      </c>
-      <c r="J13" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" ht="45" x14ac:dyDescent="0.25">
-      <c r="A14">
-        <v>222</v>
-      </c>
-      <c r="B14">
-        <v>1</v>
-      </c>
-      <c r="C14">
-        <v>1</v>
-      </c>
-      <c r="D14" t="s">
-        <v>19</v>
-      </c>
-      <c r="E14">
-        <v>1</v>
-      </c>
-      <c r="F14">
-        <v>2</v>
-      </c>
-      <c r="H14" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="J14" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A15">
-        <v>222</v>
-      </c>
-      <c r="B15">
-        <v>1</v>
-      </c>
-      <c r="C15">
-        <v>1</v>
-      </c>
-      <c r="D15" t="s">
-        <v>15</v>
-      </c>
-      <c r="E15">
-        <v>2</v>
-      </c>
-      <c r="H15" t="s">
-        <v>36</v>
-      </c>
-      <c r="J15" t="s">
-        <v>15</v>
+      <c r="H20" t="s">
+        <v>45</v>
+      </c>
+      <c r="K20">
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
complete quests with no rewards so far
</commit_message>
<xml_diff>
--- a/data/quest_dialogues_data.xlsx
+++ b/data/quest_dialogues_data.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marcin\Desktop\pygame\Kolo_game\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marcin\Desktop\KOLO\Kolo_game\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{330855B8-B28E-41C8-AA7B-2B1C4466AF31}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{497E5CFC-5E4E-41C2-9DD7-217197907891}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -159,9 +159,6 @@
     <t>Snorlax:    Oh…. Shit....</t>
   </si>
   <si>
-    <t>Snorlax:    1. Cool, here's cash.</t>
-  </si>
-  <si>
     <t>2. Gold+=100;Item#20</t>
   </si>
   <si>
@@ -181,6 +178,9 @@
   </si>
   <si>
     <t>Me:    See Ya later my friend!</t>
+  </si>
+  <si>
+    <t>Snorlax:    Cool, here's cash.</t>
   </si>
 </sst>
 </file>
@@ -505,7 +505,7 @@
   <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -562,7 +562,7 @@
         <v>0</v>
       </c>
       <c r="C3">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D3" t="s">
         <v>24</v>
@@ -624,7 +624,7 @@
   <dimension ref="A1:K20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="H18" sqref="H18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -785,7 +785,7 @@
         <v>5</v>
       </c>
       <c r="H6" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="K6">
         <v>1</v>
@@ -808,7 +808,7 @@
         <v>6</v>
       </c>
       <c r="H7" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="K7">
         <v>2</v>
@@ -831,7 +831,7 @@
         <v>7</v>
       </c>
       <c r="H8" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="K8">
         <v>1</v>
@@ -952,10 +952,10 @@
         <v>4</v>
       </c>
       <c r="H13" s="1" t="s">
-        <v>41</v>
+        <v>48</v>
       </c>
       <c r="I13" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="K13">
         <v>1</v>
@@ -981,7 +981,7 @@
         <v>39</v>
       </c>
       <c r="I14" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="K14">
         <v>2</v>
@@ -1007,7 +1007,7 @@
         <v>40</v>
       </c>
       <c r="I15" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="K15">
         <v>3</v>
@@ -1128,7 +1128,7 @@
         <v>3</v>
       </c>
       <c r="H20" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="K20">
         <v>2</v>

</xml_diff>